<commit_message>
Update data.xlsx from Excel Data Explorer
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -465,7 +465,7 @@
         <v>3/10/25</v>
       </c>
       <c r="F3" t="str">
-        <v>No</v>
+        <v>yes</v>
       </c>
       <c r="G3" t="str">
         <v>murshad</v>
@@ -491,7 +491,7 @@
         <v>No</v>
       </c>
       <c r="G4" t="str">
-        <v xml:space="preserve">incomplete record </v>
+        <v>kamyab</v>
       </c>
     </row>
     <row r="5">

</xml_diff>